<commit_message>
Reorganize testing results and add heat map.
</commit_message>
<xml_diff>
--- a/ImagePipeline_results.xlsx
+++ b/ImagePipeline_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t xml:space="preserve">Outer Parallelism and Configuration</t>
   </si>
@@ -44,43 +44,49 @@
     <t xml:space="preserve">number of images</t>
   </si>
   <si>
-    <t xml:space="preserve">1 (1|56)</t>
+    <t xml:space="preserve">1 (1|108)</t>
   </si>
   <si>
-    <t xml:space="preserve">2(2|28)</t>
+    <t xml:space="preserve">2(2|54)</t>
   </si>
   <si>
-    <t xml:space="preserve">4 (4|14)</t>
+    <t xml:space="preserve">4 (4|27)</t>
   </si>
   <si>
-    <t xml:space="preserve">8 (8|7)</t>
+    <t xml:space="preserve">8 (8|13,14)</t>
   </si>
   <si>
-    <t xml:space="preserve">16 (16|4,5)</t>
+    <t xml:space="preserve">16 (16|6,7)</t>
   </si>
   <si>
-    <t xml:space="preserve">32(32|(1,2)</t>
+    <t xml:space="preserve">32(32|(3,4)</t>
   </si>
   <si>
-    <t xml:space="preserve">56 (56|1)</t>
+    <t xml:space="preserve">54 (54|2)</t>
   </si>
   <si>
-    <t xml:space="preserve">100(56|1 or 1|(1,2))</t>
+    <t xml:space="preserve">100 (100|1,2)</t>
   </si>
   <si>
-    <t xml:space="preserve">128 (</t>
+    <t xml:space="preserve">128 (108|1 &amp; 20|5,6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">256 (108|1 &amp; 40|2,3)</t>
   </si>
   <si>
     <t xml:space="preserve">Julia|TBB</t>
   </si>
   <si>
-    <t xml:space="preserve">Juli|OpenMP</t>
+    <t xml:space="preserve">Julia|OpenMP</t>
   </si>
   <si>
     <t xml:space="preserve">OpenMP|TBB</t>
   </si>
   <si>
     <t xml:space="preserve">OpenMP|OpenMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weak Scaling</t>
   </si>
 </sst>
 </file>
@@ -91,7 +97,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -124,6 +130,13 @@
       <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
@@ -206,7 +219,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,6 +250,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -315,7 +332,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2233,11 +2250,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="19739324"/>
-        <c:axId val="29072859"/>
+        <c:axId val="70580563"/>
+        <c:axId val="58200987"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19739324"/>
+        <c:axId val="70580563"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2269,14 +2286,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29072859"/>
+        <c:crossAx val="58200987"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29072859"/>
+        <c:axId val="58200987"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2315,7 +2332,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19739324"/>
+        <c:crossAx val="70580563"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2367,7 +2384,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2455,34 +2472,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1 (1|56)</c:v>
+                  <c:v>1 (1|108)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2(2|28)</c:v>
+                  <c:v>2(2|54)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 (4|14)</c:v>
+                  <c:v>4 (4|27)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8 (8|7)</c:v>
+                  <c:v>8 (8|13,14)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16 (16|4,5)</c:v>
+                  <c:v>16 (16|6,7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32(32|(1,2)</c:v>
+                  <c:v>32(32|(3,4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56 (56|1)</c:v>
+                  <c:v>54 (54|2)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100(56|1 or 1|(1,2))</c:v>
+                  <c:v>100 (100|1,2)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>128 (</c:v>
+                  <c:v>128 (108|1 &amp; 20|5,6)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256</c:v>
+                  <c:v>256 (108|1 &amp; 40|2,3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2537,7 +2554,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Juli|OpenMP</c:v>
+                  <c:v>Julia|OpenMP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2578,34 +2595,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1 (1|56)</c:v>
+                  <c:v>1 (1|108)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2(2|28)</c:v>
+                  <c:v>2(2|54)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 (4|14)</c:v>
+                  <c:v>4 (4|27)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8 (8|7)</c:v>
+                  <c:v>8 (8|13,14)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16 (16|4,5)</c:v>
+                  <c:v>16 (16|6,7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32(32|(1,2)</c:v>
+                  <c:v>32(32|(3,4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56 (56|1)</c:v>
+                  <c:v>54 (54|2)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100(56|1 or 1|(1,2))</c:v>
+                  <c:v>100 (100|1,2)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>128 (</c:v>
+                  <c:v>128 (108|1 &amp; 20|5,6)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256</c:v>
+                  <c:v>256 (108|1 &amp; 40|2,3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2701,34 +2718,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1 (1|56)</c:v>
+                  <c:v>1 (1|108)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2(2|28)</c:v>
+                  <c:v>2(2|54)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 (4|14)</c:v>
+                  <c:v>4 (4|27)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8 (8|7)</c:v>
+                  <c:v>8 (8|13,14)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16 (16|4,5)</c:v>
+                  <c:v>16 (16|6,7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32(32|(1,2)</c:v>
+                  <c:v>32(32|(3,4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56 (56|1)</c:v>
+                  <c:v>54 (54|2)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100(56|1 or 1|(1,2))</c:v>
+                  <c:v>100 (100|1,2)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>128 (</c:v>
+                  <c:v>128 (108|1 &amp; 20|5,6)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256</c:v>
+                  <c:v>256 (108|1 &amp; 40|2,3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2824,34 +2841,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1 (1|56)</c:v>
+                  <c:v>1 (1|108)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2(2|28)</c:v>
+                  <c:v>2(2|54)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 (4|14)</c:v>
+                  <c:v>4 (4|27)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8 (8|7)</c:v>
+                  <c:v>8 (8|13,14)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16 (16|4,5)</c:v>
+                  <c:v>16 (16|6,7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32(32|(1,2)</c:v>
+                  <c:v>32(32|(3,4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56 (56|1)</c:v>
+                  <c:v>54 (54|2)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100(56|1 or 1|(1,2))</c:v>
+                  <c:v>100 (100|1,2)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>128 (</c:v>
+                  <c:v>128 (108|1 &amp; 20|5,6)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256</c:v>
+                  <c:v>256 (108|1 &amp; 40|2,3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2905,11 +2922,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="83856369"/>
-        <c:axId val="19406021"/>
+        <c:axId val="83006050"/>
+        <c:axId val="34127490"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83856369"/>
+        <c:axId val="83006050"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2941,14 +2958,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19406021"/>
+        <c:crossAx val="34127490"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19406021"/>
+        <c:axId val="34127490"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2987,7 +3004,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83856369"/>
+        <c:crossAx val="83006050"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3039,7 +3056,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3076,7 +3093,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$29</c:f>
+              <c:f>Sheet3!$A$29:$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3121,34 +3138,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1 (1|56)</c:v>
+                  <c:v>1 (1|108)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2(2|28)</c:v>
+                  <c:v>2(2|54)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 (4|14)</c:v>
+                  <c:v>4 (4|27)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8 (8|7)</c:v>
+                  <c:v>8 (8|13,14)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16 (16|4,5)</c:v>
+                  <c:v>16 (16|6,7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32(32|(1,2)</c:v>
+                  <c:v>32(32|(3,4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56 (56|1)</c:v>
+                  <c:v>54 (54|2)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100(56|1 or 1|(1,2))</c:v>
+                  <c:v>100 (100|1,2)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>128 (</c:v>
+                  <c:v>128 (108|1 &amp; 20|5,6)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256</c:v>
+                  <c:v>256 (108|1 &amp; 40|2,3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3199,11 +3216,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$30</c:f>
+              <c:f>Sheet3!$A$30:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Juli|OpenMP</c:v>
+                  <c:v>Julia|OpenMP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3244,34 +3261,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1 (1|56)</c:v>
+                  <c:v>1 (1|108)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2(2|28)</c:v>
+                  <c:v>2(2|54)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 (4|14)</c:v>
+                  <c:v>4 (4|27)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8 (8|7)</c:v>
+                  <c:v>8 (8|13,14)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16 (16|4,5)</c:v>
+                  <c:v>16 (16|6,7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32(32|(1,2)</c:v>
+                  <c:v>32(32|(3,4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56 (56|1)</c:v>
+                  <c:v>54 (54|2)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100(56|1 or 1|(1,2))</c:v>
+                  <c:v>100 (100|1,2)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>128 (</c:v>
+                  <c:v>128 (108|1 &amp; 20|5,6)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256</c:v>
+                  <c:v>256 (108|1 &amp; 40|2,3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3322,7 +3339,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$31</c:f>
+              <c:f>Sheet3!$A$31:$A$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3367,34 +3384,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1 (1|56)</c:v>
+                  <c:v>1 (1|108)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2(2|28)</c:v>
+                  <c:v>2(2|54)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 (4|14)</c:v>
+                  <c:v>4 (4|27)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8 (8|7)</c:v>
+                  <c:v>8 (8|13,14)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16 (16|4,5)</c:v>
+                  <c:v>16 (16|6,7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32(32|(1,2)</c:v>
+                  <c:v>32(32|(3,4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56 (56|1)</c:v>
+                  <c:v>54 (54|2)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100(56|1 or 1|(1,2))</c:v>
+                  <c:v>100 (100|1,2)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>128 (</c:v>
+                  <c:v>128 (108|1 &amp; 20|5,6)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256</c:v>
+                  <c:v>256 (108|1 &amp; 40|2,3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3445,7 +3462,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$32</c:f>
+              <c:f>Sheet3!$A$32:$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3490,34 +3507,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1 (1|56)</c:v>
+                  <c:v>1 (1|108)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2(2|28)</c:v>
+                  <c:v>2(2|54)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 (4|14)</c:v>
+                  <c:v>4 (4|27)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8 (8|7)</c:v>
+                  <c:v>8 (8|13,14)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16 (16|4,5)</c:v>
+                  <c:v>16 (16|6,7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32(32|(1,2)</c:v>
+                  <c:v>32(32|(3,4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56 (56|1)</c:v>
+                  <c:v>54 (54|2)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100(56|1 or 1|(1,2))</c:v>
+                  <c:v>100 (100|1,2)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>128 (</c:v>
+                  <c:v>128 (108|1 &amp; 20|5,6)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256</c:v>
+                  <c:v>256 (108|1 &amp; 40|2,3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3571,11 +3588,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="99356473"/>
-        <c:axId val="30000463"/>
+        <c:axId val="93924109"/>
+        <c:axId val="78330977"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99356473"/>
+        <c:axId val="93924109"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3603,14 +3620,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30000463"/>
+        <c:crossAx val="78330977"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30000463"/>
+        <c:axId val="78330977"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3647,7 +3664,415 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99356473"/>
+        <c:crossAx val="93924109"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Weak Scaling Testing Results</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OpenMP|TBB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="0.00" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$28:$K$28</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1 (1|108)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2(2|54)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4 (4|27)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 (8|13,14)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16 (16|6,7)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32(32|(3,4)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54 (54|2)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100 (100|1,2)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128 (108|1 &amp; 20|5,6)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>256 (108|1 &amp; 40|2,3)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$31:$K$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.38375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.313125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2753125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.242777777777778</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2354</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.247265625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23859375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OpenMP|OpenMP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="0.00" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$28:$K$28</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1 (1|108)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2(2|54)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4 (4|27)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 (8|13,14)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16 (16|6,7)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32(32|(3,4)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54 (54|2)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100 (100|1,2)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128 (108|1 &amp; 20|5,6)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>256 (108|1 &amp; 40|2,3)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$32:$K$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.653125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.618125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.606296296296296</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.612</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.615859375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6155859375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="46410780"/>
+        <c:axId val="43429942"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="46410780"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="43429942"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43429942"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="46410780"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3706,9 +4131,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>279000</xdr:colOff>
+      <xdr:colOff>278280</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3717,7 +4142,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9492120" y="5416200"/>
-        <a:ext cx="10096920" cy="5917320"/>
+        <a:ext cx="10096200" cy="5916600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3734,16 +4159,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>130320</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>182520</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>758160</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>529560</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>370080</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>111600</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3751,8 +4176,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9688320" y="3693960"/>
-        <a:ext cx="8376120" cy="5402880"/>
+        <a:off x="14646240" y="3737160"/>
+        <a:ext cx="9165960" cy="5395680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3764,16 +4189,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>737280</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>48960</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>531360</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>748800</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3781,12 +4206,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2389320" y="6535440"/>
-        <a:ext cx="6873840" cy="5669280"/>
+        <a:off x="6782400" y="6562440"/>
+        <a:ext cx="6871320" cy="5668920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>104760</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>63000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>439560</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="104760" y="6476400"/>
+        <a:ext cx="6232680" cy="4798440"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3802,7 +4257,7 @@
   </sheetPr>
   <dimension ref="H15:AM26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J50" activeCellId="0" sqref="J50"/>
     </sheetView>
   </sheetViews>
@@ -4444,17 +4899,24 @@
   </sheetPr>
   <dimension ref="A10:P32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="10.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="7" style="0" width="10.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="19.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="19.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="10.67"/>
   </cols>
   <sheetData>
     <row r="10" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4471,7 +4933,7 @@
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="0" t="s">
         <v>7</v>
       </c>
@@ -4499,13 +4961,13 @@
       <c r="O11" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="P11" s="0" t="n">
-        <v>256</v>
+      <c r="P11" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>1.34</v>
@@ -4540,7 +5002,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>1.33</v>
@@ -4575,7 +5037,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>1.34</v>
@@ -4610,7 +5072,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>1.33</v>
@@ -4673,6 +5135,11 @@
       </c>
       <c r="P17" s="0" t="n">
         <v>256</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4717,186 +5184,186 @@
       <c r="J28" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K28" s="0" t="n">
-        <v>256</v>
+      <c r="K28" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="8" t="n">
+        <v>17</v>
+      </c>
+      <c r="B29" s="9" t="n">
         <f aca="false">G12/G17</f>
         <v>1.34</v>
       </c>
-      <c r="C29" s="8" t="n">
+      <c r="C29" s="9" t="n">
         <f aca="false">H12/H17</f>
         <v>0.73</v>
       </c>
-      <c r="D29" s="8" t="n">
+      <c r="D29" s="9" t="n">
         <f aca="false">I12/I17</f>
         <v>0.525</v>
       </c>
-      <c r="E29" s="8" t="n">
+      <c r="E29" s="9" t="n">
         <f aca="false">J12/J17</f>
         <v>0.38375</v>
       </c>
-      <c r="F29" s="8" t="n">
+      <c r="F29" s="9" t="n">
         <f aca="false">K12/K17</f>
         <v>0.313125</v>
       </c>
-      <c r="G29" s="8" t="n">
+      <c r="G29" s="9" t="n">
         <f aca="false">L12/L17</f>
         <v>0.2753125</v>
       </c>
-      <c r="H29" s="8" t="n">
+      <c r="H29" s="9" t="n">
         <f aca="false">M12/M17</f>
         <v>0.242777777777778</v>
       </c>
-      <c r="I29" s="8" t="n">
+      <c r="I29" s="9" t="n">
         <f aca="false">N12/N17</f>
         <v>0.2354</v>
       </c>
-      <c r="J29" s="8" t="n">
+      <c r="J29" s="9" t="n">
         <f aca="false">O12/O17</f>
         <v>0.247265625</v>
       </c>
-      <c r="K29" s="8" t="n">
+      <c r="K29" s="9" t="n">
         <f aca="false">P12/P17</f>
         <v>0.23859375</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="8" t="n">
+        <v>18</v>
+      </c>
+      <c r="B30" s="9" t="n">
         <f aca="false">G13/G17</f>
         <v>1.33</v>
       </c>
-      <c r="C30" s="8" t="n">
+      <c r="C30" s="9" t="n">
         <f aca="false">H13/H17</f>
         <v>0.96</v>
       </c>
-      <c r="D30" s="8" t="n">
+      <c r="D30" s="9" t="n">
         <f aca="false">I13/I17</f>
         <v>0.75</v>
       </c>
-      <c r="E30" s="8" t="n">
+      <c r="E30" s="9" t="n">
         <f aca="false">J13/J17</f>
         <v>0.68875</v>
       </c>
-      <c r="F30" s="8" t="n">
+      <c r="F30" s="9" t="n">
         <f aca="false">K13/K17</f>
         <v>0.653125</v>
       </c>
-      <c r="G30" s="8" t="n">
+      <c r="G30" s="9" t="n">
         <f aca="false">L13/L17</f>
         <v>0.618125</v>
       </c>
-      <c r="H30" s="8" t="n">
+      <c r="H30" s="9" t="n">
         <f aca="false">M13/M17</f>
         <v>0.606296296296296</v>
       </c>
-      <c r="I30" s="8" t="n">
+      <c r="I30" s="9" t="n">
         <f aca="false">N13/N17</f>
         <v>0.612</v>
       </c>
-      <c r="J30" s="8" t="n">
+      <c r="J30" s="9" t="n">
         <f aca="false">O13/O17</f>
         <v>0.615859375</v>
       </c>
-      <c r="K30" s="8" t="n">
+      <c r="K30" s="9" t="n">
         <f aca="false">P13/P17</f>
         <v>0.6155859375</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="8" t="n">
+        <v>19</v>
+      </c>
+      <c r="B31" s="9" t="n">
         <f aca="false">G14/G17</f>
         <v>1.34</v>
       </c>
-      <c r="C31" s="8" t="n">
+      <c r="C31" s="9" t="n">
         <f aca="false">H14/H17</f>
         <v>0.73</v>
       </c>
-      <c r="D31" s="8" t="n">
+      <c r="D31" s="9" t="n">
         <f aca="false">I14/I17</f>
         <v>0.525</v>
       </c>
-      <c r="E31" s="8" t="n">
+      <c r="E31" s="9" t="n">
         <f aca="false">J14/J17</f>
         <v>0.38375</v>
       </c>
-      <c r="F31" s="8" t="n">
+      <c r="F31" s="9" t="n">
         <f aca="false">K14/K17</f>
         <v>0.313125</v>
       </c>
-      <c r="G31" s="8" t="n">
+      <c r="G31" s="9" t="n">
         <f aca="false">L14/L17</f>
         <v>0.2753125</v>
       </c>
-      <c r="H31" s="8" t="n">
+      <c r="H31" s="9" t="n">
         <f aca="false">M14/M17</f>
         <v>0.242777777777778</v>
       </c>
-      <c r="I31" s="8" t="n">
+      <c r="I31" s="9" t="n">
         <f aca="false">N14/N17</f>
         <v>0.2354</v>
       </c>
-      <c r="J31" s="8" t="n">
+      <c r="J31" s="9" t="n">
         <f aca="false">O14/O17</f>
         <v>0.247265625</v>
       </c>
-      <c r="K31" s="8" t="n">
+      <c r="K31" s="9" t="n">
         <f aca="false">P14/P17</f>
         <v>0.23859375</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="B32" s="9" t="n">
         <f aca="false">G15/G17</f>
         <v>1.33</v>
       </c>
-      <c r="C32" s="8" t="n">
+      <c r="C32" s="9" t="n">
         <f aca="false">H15/H17</f>
         <v>0.96</v>
       </c>
-      <c r="D32" s="8" t="n">
+      <c r="D32" s="9" t="n">
         <f aca="false">I15/I17</f>
         <v>0.75</v>
       </c>
-      <c r="E32" s="8" t="n">
+      <c r="E32" s="9" t="n">
         <f aca="false">J15/J17</f>
         <v>0.68875</v>
       </c>
-      <c r="F32" s="8" t="n">
+      <c r="F32" s="9" t="n">
         <f aca="false">K15/K17</f>
         <v>0.653125</v>
       </c>
-      <c r="G32" s="8" t="n">
+      <c r="G32" s="9" t="n">
         <f aca="false">L15/L17</f>
         <v>0.618125</v>
       </c>
-      <c r="H32" s="8" t="n">
+      <c r="H32" s="9" t="n">
         <f aca="false">M15/M17</f>
         <v>0.606296296296296</v>
       </c>
-      <c r="I32" s="8" t="n">
+      <c r="I32" s="9" t="n">
         <f aca="false">N15/N17</f>
         <v>0.612</v>
       </c>
-      <c r="J32" s="8" t="n">
+      <c r="J32" s="9" t="n">
         <f aca="false">O15/O17</f>
         <v>0.615859375</v>
       </c>
-      <c r="K32" s="8" t="n">
+      <c r="K32" s="9" t="n">
         <f aca="false">P15/P17</f>
         <v>0.6155859375</v>
       </c>

</xml_diff>